<commit_message>
tema 2 parcial 1
</commit_message>
<xml_diff>
--- a/fund_math.xlsx
+++ b/fund_math.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\3_funda_math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11003C63-46CA-4FCE-9212-C932E6090AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D68C70-9EFE-41A6-AAB8-CEC881EC0DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fund_math" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Nombre</t>
   </si>
@@ -131,12 +131,33 @@
   </si>
   <si>
     <t>keiner.zapata@udea.edu.co</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>tf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -970,10 +991,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -981,15 +1004,36 @@
     <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -997,7 +1041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1005,7 +1049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1021,7 +1065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1029,7 +1073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1037,7 +1081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1045,7 +1089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1053,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1061,7 +1105,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1069,7 +1113,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1085,7 +1129,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1093,7 +1137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1101,7 +1145,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
mejoras a la valoración de los puntos del primer parcial y enfasis en la modelación matemática
</commit_message>
<xml_diff>
--- a/fund_math.xlsx
+++ b/fund_math.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\3_funda_math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D68C70-9EFE-41A6-AAB8-CEC881EC0DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC682A-E17B-4365-A65E-64C2276843EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Nombre</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>tf</t>
+  </si>
+  <si>
+    <t>zapata keiner</t>
   </si>
 </sst>
 </file>
@@ -995,7 +998,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1170,6 +1173,9 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
       <c r="B19" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
creación de unidad didáctica sobre productos notables y factorización
</commit_message>
<xml_diff>
--- a/fund_math.xlsx
+++ b/fund_math.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\3_funda_math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC682A-E17B-4365-A65E-64C2276843EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24550CEF-FDE8-4565-AA4B-51C8311A0BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Nombre</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>zapata keiner</t>
+  </si>
+  <si>
+    <t>horas de faltas</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,6 +478,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -638,8 +647,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -995,19 +1008,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.81640625" customWidth="1"/>
     <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1035,152 +1049,188 @@
       <c r="I1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
       </c>
+      <c r="J19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>